<commit_message>
Se actualiza Readme y artefactos
</commit_message>
<xml_diff>
--- a/artefactos/RGB/train_results/CNN_Classifier.xlsx
+++ b/artefactos/RGB/train_results/CNN_Classifier.xlsx
@@ -615,16 +615,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>0.1011</v>
+        <v>0.15429999999999999</v>
       </c>
       <c r="C2" s="2">
-        <v>1.9599999999999999E-2</v>
+        <v>1.46E-2</v>
       </c>
       <c r="D2" s="2">
-        <v>0.99650000000000005</v>
+        <v>0.99780000000000002</v>
       </c>
       <c r="E2" s="2">
-        <v>0.99650000000000005</v>
+        <v>0.99780000000000002</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -632,16 +632,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>1.55E-2</v>
+        <v>1.47E-2</v>
       </c>
       <c r="C3" s="1">
-        <v>2.2100000000000002E-2</v>
+        <v>2.0299999999999999E-2</v>
       </c>
       <c r="D3" s="2">
-        <v>0.99580000000000002</v>
+        <v>0.996</v>
       </c>
       <c r="E3" s="2">
-        <v>0.99580000000000002</v>
+        <v>0.996</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -649,16 +649,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>1.6299999999999999E-2</v>
+        <v>1.0200000000000001E-2</v>
       </c>
       <c r="C4" s="2">
-        <v>6.8400000000000002E-2</v>
+        <v>1.44E-2</v>
       </c>
       <c r="D4" s="2">
-        <v>0.99119999999999997</v>
+        <v>0.99709999999999999</v>
       </c>
       <c r="E4" s="2">
-        <v>0.99119999999999997</v>
+        <v>0.99709999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -666,16 +666,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>1.8200000000000001E-2</v>
+        <v>0.124</v>
       </c>
       <c r="C5" s="2">
-        <v>2.5399999999999999E-2</v>
+        <v>6.7100000000000007E-2</v>
       </c>
       <c r="D5" s="2">
-        <v>0.99490000000000001</v>
+        <v>0.99139999999999995</v>
       </c>
       <c r="E5" s="2">
-        <v>0.99490000000000001</v>
+        <v>0.99139999999999995</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -683,16 +683,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>1.2800000000000001E-2</v>
+        <v>2.0500000000000001E-2</v>
       </c>
       <c r="C6" s="2">
-        <v>2.0400000000000001E-2</v>
+        <v>2.1899999999999999E-2</v>
       </c>
       <c r="D6" s="2">
-        <v>0.99419999999999997</v>
+        <v>0.996</v>
       </c>
       <c r="E6" s="2">
-        <v>0.99419999999999997</v>
+        <v>0.996</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -700,16 +700,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>8.6999999999999994E-3</v>
+        <v>8.3000000000000001E-3</v>
       </c>
       <c r="C7" s="2">
-        <v>2.18E-2</v>
+        <v>1.8800000000000001E-2</v>
       </c>
       <c r="D7" s="2">
-        <v>0.99680000000000002</v>
+        <v>0.99639999999999995</v>
       </c>
       <c r="E7" s="2">
-        <v>0.99680000000000002</v>
+        <v>0.99639999999999995</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -717,16 +717,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>2.4199999999999999E-2</v>
+        <v>3.8999999999999998E-3</v>
       </c>
       <c r="C8" s="2">
-        <v>2.4500000000000001E-2</v>
+        <v>0.24</v>
       </c>
       <c r="D8" s="2">
-        <v>0.99619999999999997</v>
+        <v>0.996</v>
       </c>
       <c r="E8" s="2">
-        <v>0.99619999999999997</v>
+        <v>0.996</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -734,16 +734,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>7.3000000000000001E-3</v>
+        <v>1.09E-2</v>
       </c>
       <c r="C9" s="2">
-        <v>2.4899999999999999E-2</v>
+        <v>1.9400000000000001E-2</v>
       </c>
       <c r="D9" s="2">
-        <v>0.99650000000000005</v>
+        <v>0.99519999999999997</v>
       </c>
       <c r="E9" s="2">
-        <v>0.99650000000000005</v>
+        <v>0.99519999999999997</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -751,16 +751,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>6.1000000000000004E-3</v>
+        <v>9.7999999999999997E-3</v>
       </c>
       <c r="C10" s="2">
-        <v>2.0299999999999999E-2</v>
+        <v>2.46E-2</v>
       </c>
       <c r="D10" s="2">
-        <v>0.99760000000000004</v>
+        <v>0.99629999999999996</v>
       </c>
       <c r="E10" s="2">
-        <v>0.99760000000000004</v>
+        <v>0.99629999999999996</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -768,16 +768,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>2.5999999999999999E-3</v>
+        <v>6.1000000000000004E-3</v>
       </c>
       <c r="C11" s="2">
-        <v>1.9800000000000002E-2</v>
+        <v>2.06E-2</v>
       </c>
       <c r="D11" s="2">
-        <v>0.99590000000000001</v>
+        <v>0.99629999999999996</v>
       </c>
       <c r="E11" s="2">
-        <v>0.99590000000000001</v>
+        <v>0.99629999999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>